<commit_message>
add parseCompUnit to parseCond
</commit_message>
<xml_diff>
--- a/FIRST.xlsx
+++ b/FIRST.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\document\CQULAB\compilerlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E5E747-D0AB-41CE-8670-F60CC25F7A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE8B421-66C5-42BD-AC72-7A187D28B6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="53">
   <si>
     <t>CompUnit</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -186,6 +197,21 @@
   </si>
   <si>
     <t>Ident</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ident </t>
+  </si>
+  <si>
+    <t>;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lval</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>=</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -528,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE6"/>
+  <dimension ref="A1:AE17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -544,6 +570,7 @@
     <col min="6" max="7" width="14.77734375" customWidth="1"/>
     <col min="12" max="12" width="12.44140625" customWidth="1"/>
     <col min="13" max="13" width="13.109375" customWidth="1"/>
+    <col min="19" max="19" width="24.44140625" customWidth="1"/>
     <col min="20" max="20" width="9.77734375" customWidth="1"/>
     <col min="21" max="21" width="11.77734375" customWidth="1"/>
     <col min="22" max="22" width="9.6640625" customWidth="1"/>
@@ -688,6 +715,15 @@
       <c r="P2" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="Q2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="T2" s="2" t="s">
         <v>31</v>
       </c>
@@ -699,6 +735,30 @@
       </c>
       <c r="W2" t="s">
         <v>37</v>
+      </c>
+      <c r="X2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -726,6 +786,12 @@
       <c r="P3" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="Q3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="T3" s="2" t="s">
         <v>32</v>
       </c>
@@ -737,6 +803,30 @@
       </c>
       <c r="W3" s="2" t="s">
         <v>39</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
@@ -752,6 +842,12 @@
       <c r="P4" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="Q4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="U4" s="2" t="s">
         <v>32</v>
       </c>
@@ -760,16 +856,231 @@
       </c>
       <c r="W4" t="s">
         <v>38</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="P5" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="Q5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="P6" s="2" t="s">
         <v>26</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>37</v>
+      </c>
+      <c r="R6" t="s">
+        <v>37</v>
+      </c>
+      <c r="V6" t="s">
+        <v>37</v>
+      </c>
+      <c r="X6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="P7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="P8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>38</v>
+      </c>
+      <c r="R8" t="s">
+        <v>38</v>
+      </c>
+      <c r="V8" t="s">
+        <v>38</v>
+      </c>
+      <c r="X8" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="P9" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="P11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="P12" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="P13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="P14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="S14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="P15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="P16" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P17" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>